<commit_message>
filter table sust_Domain and tendency buttons
</commit_message>
<xml_diff>
--- a/DB_ImportFields.xlsx
+++ b/DB_ImportFields.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="860" windowWidth="24720" windowHeight="16580" tabRatio="678" activeTab="3"/>
+    <workbookView xWindow="880" yWindow="860" windowWidth="24720" windowHeight="16580" tabRatio="678" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="allg" sheetId="8" r:id="rId1"/>
-    <sheet name="SustDomain" sheetId="17" r:id="rId2"/>
-    <sheet name="SustCat" sheetId="15" r:id="rId3"/>
-    <sheet name="Tags" sheetId="4" r:id="rId4"/>
-    <sheet name="Country" sheetId="26" r:id="rId5"/>
-    <sheet name="Subcat_DE" sheetId="14" r:id="rId6"/>
+    <sheet name="SustTendency" sheetId="27" r:id="rId2"/>
+    <sheet name="SustDomain" sheetId="17" r:id="rId3"/>
+    <sheet name="SustCat" sheetId="15" r:id="rId4"/>
+    <sheet name="Tags" sheetId="4" r:id="rId5"/>
+    <sheet name="Country" sheetId="26" r:id="rId6"/>
+    <sheet name="Subcat_DE" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Subcat_DE!$A$1:$F$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tags!$A$1:$E$32</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Subcat_DE!$B:$D</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Subcat_DE!$A$1:$F$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Tags!$A$1:$E$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Subcat_DE!$B:$D</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="928">
   <si>
     <t>People</t>
   </si>
@@ -2823,6 +2824,9 @@
   </si>
   <si>
     <t>Involvement In third World Debt</t>
+  </si>
+  <si>
+    <t>Controversial</t>
   </si>
 </sst>
 </file>
@@ -4160,10 +4164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4181,11 +4185,11 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D6" si="0">LEN(B3)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4193,11 +4197,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4205,35 +4209,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>927</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7">
-        <f>LEN(B7)</f>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4249,359 +4229,80 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>133</v>
       </c>
       <c r="B1" t="s">
         <v>132</v>
       </c>
-      <c r="C1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <f>LEN(B3)</f>
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <f>LEN(C3)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f t="shared" ref="D3:D6" si="0">LEN(B3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:G16" si="0">LEN(B4)</f>
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <f>LEN(B17)</f>
-        <v>31</v>
-      </c>
-      <c r="G17">
-        <f>LEN(C17)</f>
-        <v>31</v>
+        <f>LEN(B7)</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4617,17 +4318,385 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>LEN(B3)</f>
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <f>LEN(C3)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:G16" si="0">LEN(B4)</f>
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <f>LEN(B17)</f>
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <f>LEN(C17)</f>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -5298,132 +5367,6 @@
       </c>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="41"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="41"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="41"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="41"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="41"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="41"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="41"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="41"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="41"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="41"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="41"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="41"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="41"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="41"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="41"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="41"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="41"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="41"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:E32"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5436,7 +5379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F251"/>
   <sheetViews>
@@ -9956,7 +9899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.39997558519241921"/>

</xml_diff>

<commit_message>
adapt to model changes: domain and tendency in ImpactEvent
</commit_message>
<xml_diff>
--- a/DB_ImportFields.xlsx
+++ b/DB_ImportFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="860" windowWidth="24720" windowHeight="16580" tabRatio="678" activeTab="3"/>
+    <workbookView xWindow="580" yWindow="0" windowWidth="24720" windowHeight="16580" tabRatio="678" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="allg" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="927">
   <si>
     <t>People</t>
   </si>
@@ -2734,9 +2734,6 @@
   </si>
   <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>10;1</t>
   </si>
   <si>
     <t>1;4;7</t>
@@ -4080,14 +4077,14 @@
         <v>46</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="6" t="s">
+        <v>911</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>912</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>913</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -4209,7 +4206,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -4320,7 +4317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4348,10 +4345,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -4370,10 +4367,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4414,10 +4411,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C6" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -4436,10 +4433,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -4480,10 +4477,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -4502,10 +4499,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C10" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -4546,10 +4543,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C12" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -4568,10 +4565,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C13" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -4612,10 +4609,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C15" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -4634,10 +4631,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C16" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -4691,12 +4688,12 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4743,7 +4740,7 @@
         <v>128</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>128</v>
@@ -4762,7 +4759,7 @@
         <v>134</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>134</v>
@@ -4781,7 +4778,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>23</v>
@@ -4819,7 +4816,7 @@
         <v>892</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>892</v>
@@ -4840,7 +4837,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>13</v>
@@ -4859,7 +4856,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>18</v>
@@ -4878,7 +4875,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>20</v>
@@ -4897,7 +4894,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>19</v>
@@ -4916,7 +4913,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>8</v>
@@ -4935,7 +4932,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>887</v>
@@ -4954,7 +4951,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>888</v>
@@ -4973,7 +4970,7 @@
         <v>22</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>889</v>
@@ -5122,13 +5119,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>896</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E23" s="15"/>
       <c r="G23" s="7">
@@ -5141,7 +5138,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>896</v>
@@ -5160,13 +5157,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>896</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E25" s="15"/>
       <c r="G25" s="7">
@@ -5179,13 +5176,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>896</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E26" s="15"/>
       <c r="G26" s="7">
@@ -5198,7 +5195,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>896</v>
@@ -5217,7 +5214,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>896</v>
@@ -5236,7 +5233,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>896</v>
@@ -5277,7 +5274,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>12</v>
@@ -5312,13 +5309,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C33" s="15" t="s">
+        <v>907</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>908</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>909</v>
       </c>
       <c r="E33" s="15"/>
     </row>
@@ -5327,13 +5324,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="15" t="s">
+        <v>906</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>907</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>908</v>
-      </c>
       <c r="D34" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E34" s="15"/>
     </row>
@@ -5342,13 +5339,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E35" s="15"/>
     </row>
@@ -5357,13 +5354,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>896</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E36" s="15"/>
     </row>

</xml_diff>

<commit_message>
WIP: import excel: name tendency; table: hand pointer
</commit_message>
<xml_diff>
--- a/DB_ImportFields.xlsx
+++ b/DB_ImportFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="0" windowWidth="24720" windowHeight="16580" tabRatio="678" activeTab="2"/>
+    <workbookView xWindow="580" yWindow="0" windowWidth="24720" windowHeight="16580" tabRatio="678" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="allg" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="931">
   <si>
     <t>People</t>
   </si>
@@ -2787,9 +2787,6 @@
     <t>Involvement In third World Debt</t>
   </si>
   <si>
-    <t>Controversial</t>
-  </si>
-  <si>
     <t>People positive</t>
   </si>
   <si>
@@ -2830,6 +2827,15 @@
   </si>
   <si>
     <t>Animals</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>controversial</t>
   </si>
 </sst>
 </file>
@@ -4171,8 +4177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4190,11 +4196,11 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>928</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D5" si="0">LEN(B3)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4202,11 +4208,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>929</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4214,7 +4220,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>914</v>
+        <v>930</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -4236,7 +4242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4267,7 +4273,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -4303,7 +4309,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D7">
         <f>LEN(B7)</f>
@@ -4326,7 +4332,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4353,10 +4359,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -4375,10 +4381,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4419,10 +4425,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C6" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -4441,10 +4447,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -4485,10 +4491,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -4507,10 +4513,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -4551,10 +4557,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C12" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -4573,10 +4579,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C13" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -4617,10 +4623,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C15" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -4639,10 +4645,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C16" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -4701,7 +4707,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -5377,13 +5383,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>894</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E37" s="15"/>
     </row>
@@ -5392,13 +5398,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>894</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E38" s="15"/>
     </row>

</xml_diff>